<commit_message>
added unit tests for api
</commit_message>
<xml_diff>
--- a/backend/uploads/extracted_data.xlsx
+++ b/backend/uploads/extracted_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,578 +436,1717 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Age</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Last Name</t>
-        </is>
-      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>Department</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>Last1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>21</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Last1</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>First1</t>
+          <t>Department1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Last2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>22</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Last2</t>
-        </is>
-      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>First2</t>
+          <t>Department2</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Last3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>23</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Last3</t>
-        </is>
-      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>First3</t>
+          <t>Department3</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Last4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>24</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Last4</t>
-        </is>
-      </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>First4</t>
+          <t>Department4</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>Last5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>25</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Last5</t>
-        </is>
-      </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>First5</t>
+          <t>Department0</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>Last6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>26</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Last6</t>
-        </is>
-      </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>First6</t>
+          <t>Department1</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>Last7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
           <t>27</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Last7</t>
-        </is>
-      </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>First7</t>
+          <t>Department2</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Last8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>28</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Last8</t>
-        </is>
-      </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>First8</t>
+          <t>Department3</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>Last9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>29</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Last9</t>
-        </is>
-      </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>First9</t>
+          <t>Department4</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Last10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
           <t>30</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Last10</t>
-        </is>
-      </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>First10</t>
+          <t>Department0</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>Last11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>31</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Last11</t>
-        </is>
-      </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>First11</t>
+          <t>Department1</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Last12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>32</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Last12</t>
-        </is>
-      </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>First12</t>
+          <t>Department2</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>Last13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>33</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Last13</t>
-        </is>
-      </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>First13</t>
+          <t>Department3</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>Last14</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
           <t>34</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Last14</t>
-        </is>
-      </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>First14</t>
+          <t>Department4</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>Last15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>35</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Last15</t>
-        </is>
-      </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>First15</t>
+          <t>Department0</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>Last16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>36</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Last16</t>
-        </is>
-      </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>First16</t>
+          <t>Department1</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>Last17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
           <t>37</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Last17</t>
-        </is>
-      </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>First17</t>
+          <t>Department2</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
+          <t>Last18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
           <t>38</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Last18</t>
-        </is>
-      </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>First18</t>
+          <t>Department3</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>Last19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
           <t>39</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Last19</t>
-        </is>
-      </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>First19</t>
+          <t>Department4</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>Last20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>40</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Last20</t>
-        </is>
-      </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>First20</t>
+          <t>Department0</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>Last21</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
           <t>41</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Last21</t>
-        </is>
-      </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>First21</t>
+          <t>Department1</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>Last22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
           <t>42</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Last22</t>
-        </is>
-      </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>First22</t>
+          <t>Department2</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>Last23</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>43</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Last23</t>
-        </is>
-      </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>First23</t>
+          <t>Department3</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>Last24</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
           <t>44</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Last24</t>
-        </is>
-      </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>First24</t>
+          <t>Department4</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
+          <t>Last25</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
           <t>45</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Last25</t>
-        </is>
-      </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>First25</t>
+          <t>Department0</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
+          <t>Last26</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
           <t>46</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Last26</t>
-        </is>
-      </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>First26</t>
+          <t>Department1</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>Last27</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>47</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Last27</t>
-        </is>
-      </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>First27</t>
+          <t>Department2</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>Last28</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
           <t>48</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Last28</t>
-        </is>
-      </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>First28</t>
+          <t>Department3</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
+          <t>Last29</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
           <t>49</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Last29</t>
-        </is>
-      </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>First29</t>
+          <t>Department4</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>Last30</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>20</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Last30</t>
-        </is>
-      </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>First30</t>
+          <t>Department0</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>Last31</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
           <t>21</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Last31</t>
-        </is>
-      </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>First31</t>
+          <t>Department1</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
+          <t>Last32</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
           <t>22</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Last32</t>
-        </is>
-      </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>First32</t>
+          <t>Department2</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>Last33</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
           <t>23</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Last33</t>
-        </is>
-      </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>First33</t>
+          <t>Department3</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Last34</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Department4</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Last35</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Department0</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Last36</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Department1</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Last37</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Department2</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Last38</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Department3</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Last39</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Department4</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Last40</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Department0</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Last41</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Department1</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Last42</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Department2</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Last43</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Department3</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Last44</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Department4</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Last45</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Department0</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Last46</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Department1</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Last47</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Department2</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Last48</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Department3</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Last49</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Department4</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Last50</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Department0</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Last51</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Department1</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Last52</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Department2</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Last53</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Department3</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Last54</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Department4</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Last55</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Department0</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Last56</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Department1</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Last57</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Department2</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Last58</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Department3</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Last59</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Department4</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Last60</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Department0</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Last61</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Department1</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Last62</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Department2</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Last63</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Department3</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Last64</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Department4</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Last65</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Department0</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Last66</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Department1</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Last67</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Department2</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Last68</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Department3</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Last69</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Department4</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Last70</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Department0</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Last71</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Department1</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Last72</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Department2</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Last73</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Department3</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Last74</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Department4</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Last75</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Department0</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Last76</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Department1</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Last77</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Department2</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Last78</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Department3</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Last79</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Department4</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Last80</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Department0</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Last81</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Department1</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Last82</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Department2</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Last83</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Department3</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Last84</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Department4</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Last85</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Department0</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Last86</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Department1</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Last87</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Department2</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Last88</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Department3</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Last89</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Department4</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Last90</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Department0</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Last91</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Department1</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Last92</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Department2</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Last93</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Department3</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Last94</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Department4</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Last95</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Department0</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Last96</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Department1</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Last97</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Department2</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Last98</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Department3</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>Last99</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Department4</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Last100</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Department0</t>
         </is>
       </c>
     </row>

</xml_diff>